<commit_message>
4 SCP ready to test
</commit_message>
<xml_diff>
--- a/P05/Scrum_MICE.xlsx
+++ b/P05/Scrum_MICE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rishabh/Desktop/cse1325/P05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE6B53C-A4F2-8048-85A1-914E8DA54183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29ABD2E-668B-AB44-81C8-7742E814B955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22740" windowHeight="28300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="186">
   <si>
     <t>Product Name:</t>
   </si>
@@ -597,6 +597,9 @@
   </si>
   <si>
     <t>In Test</t>
+  </si>
+  <si>
+    <t>Create Scoop class and add constructor, addMixIn and override toString methods</t>
   </si>
 </sst>
 </file>
@@ -1347,28 +1350,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5702,7 +5705,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -5804,7 +5807,7 @@
       </c>
       <c r="B7" s="18">
         <f>COUNTA(D17:D995)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -5819,7 +5822,7 @@
       </c>
       <c r="B8" s="18">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5837,7 +5840,7 @@
       </c>
       <c r="B9" s="18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5855,7 +5858,7 @@
       </c>
       <c r="B10" s="18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5873,7 +5876,7 @@
       </c>
       <c r="B11" s="18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5891,7 +5894,7 @@
       </c>
       <c r="B12" s="18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5909,7 +5912,7 @@
       </c>
       <c r="B13" s="18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5927,7 +5930,7 @@
       </c>
       <c r="B14" s="18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="18">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6024,7 +6027,9 @@
       <c r="C20" t="s">
         <v>180</v>
       </c>
-      <c r="D20" s="26"/>
+      <c r="D20" s="27" t="s">
+        <v>185</v>
+      </c>
       <c r="E20" s="28"/>
     </row>
     <row r="21" spans="1:5">
@@ -6032,7 +6037,7 @@
         <v>5</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="D21" s="26"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="28"/>
     </row>
     <row r="22" spans="1:5">

</xml_diff>